<commit_message>
Added endpoints to readme
</commit_message>
<xml_diff>
--- a/Endpoints_and_testcases.xlsx
+++ b/Endpoints_and_testcases.xlsx
@@ -137,21 +137,11 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">{
-    "MNAME": "Dinner",
-    "MDETAILS": "All dishes relating to dinner before 9:00PM are stored here",
-    "RID": "1"
-}
+    <t xml:space="preserve">{"MNAME": "Dinner","MDETAILS": "All dishes relating to dinner before 9:00PM are stored here","RID": "1"}
 </t>
   </si>
   <si>
-    <t>{
-    "MITEMNAME": "Prime RIB",
-    "MITEMDETAILS": "Burger",
-    "MITEMPRICE": 4.95,
-    "MID": "1",
-    "RID": "1"
-}</t>
+    <t>{"MITEMNAME": "Prime RIB","MITEMDETAILS": "Burger","MITEMPRICE": 4.95,"MID": "1","RID": "1"}</t>
   </si>
 </sst>
 </file>
@@ -532,7 +522,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,7 +644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -702,7 +692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Fixes in response handling
</commit_message>
<xml_diff>
--- a/Endpoints_and_testcases.xlsx
+++ b/Endpoints_and_testcases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Endpoint</t>
   </si>
@@ -72,18 +72,6 @@
   </si>
   <si>
     <t>/menuItem</t>
-  </si>
-  <si>
-    <t>http://localhost:5000/restaurant/2</t>
-  </si>
-  <si>
-    <t>http://localhost:5000/menu/2</t>
-  </si>
-  <si>
-    <t>http://localhost:5000/menuItem/2</t>
-  </si>
-  <si>
-    <t>JSON Example</t>
   </si>
   <si>
     <t>Get menus of a restaurant using its Menu ID</t>
@@ -123,17 +111,59 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">http://localhost:5000/menuItem/2
+    <t>{"RNAME":"Jack in the Box","ADDRESS":"San Fransisco","PHONE":"500-004-3003"}</t>
+  </si>
+  <si>
+    <t>{"MITEMNAME":"PrimeRib","MITEMDETAILS":"Burger","MITEMPRICE":4.95,"MID":"1","RID":"1"}</t>
+  </si>
+  <si>
+    <t>{"Message":"Welcome to the Restaurant API V1.0."}</t>
+  </si>
+  <si>
+    <t>JSON Request</t>
+  </si>
+  <si>
+    <t>JSON Response</t>
+  </si>
+  <si>
+    <t>{"Message":"Restaurant with RID: 22 added to Table DB.","RID":22}</t>
+  </si>
+  <si>
+    <t>{"RID":"22","RNAME":"Jack in the Box","ADDRESS":"San Fransisco","PHONE":"500-004-3003"}</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/restaurant/22</t>
+  </si>
+  <si>
+    <t>{"MNAME":"Dinner","MDETAILS":"All dishes relating to dinner before 9:00PM are stored here","RID":"22"}</t>
+  </si>
+  <si>
+    <t>{"Message":"Menus with ID: 26 of Restaurant with RID: 22 added to Menus Table in DB.","MID":26,"RID":"22"}</t>
+  </si>
+  <si>
+    <t>http://localhost:5000/menu/26</t>
+  </si>
+  <si>
+    <t>{"MID":"26","MNAME":"Dinner","MDETAILS":"All dishes relating to dinner before 9:00PM are stored here","RID":"22"}</t>
+  </si>
+  <si>
+    <t>{"Message":"MenuItem with ID: 6 of Restaurant with RID: 22 added to Menus Table in DB.","MIID":6,"MID":"26","RID":"22"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://localhost:5000/menuItem/6
 </t>
   </si>
   <si>
-    <t>{"RNAME":"Jack in the Box","ADDRESS":"San Fransisco","PHONE":"500-004-3003"}</t>
-  </si>
-  <si>
-    <t>{"MITEMNAME":"PrimeRib","MITEMDETAILS":"Burger","MITEMPRICE":4.95,"MID":"1","RID":"1"}</t>
-  </si>
-  <si>
-    <t>{"MNAME":"Dinner","MDETAILS":"All dishes relating to dinner before 9:00PM are stored here","RID":"1"}</t>
+    <t>{"MIID":"6","MITEMNAME":"PrimeRib","MITEMDETAILS":"Burger","MITEMPRICE":"4.95","MID":"26","RID":"22"}</t>
+  </si>
+  <si>
+    <t>{"Message":"Menu with ID:26 deleted from DB"}</t>
+  </si>
+  <si>
+    <t>{"Message":"MenuItem with ID:6 deleted from DB"}</t>
+  </si>
+  <si>
+    <t>{"Message":"Restaurant with RID:22 deleted from DB","RID":"22"}</t>
   </si>
 </sst>
 </file>
@@ -186,17 +216,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -514,201 +550,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54694125-B7FF-44F6-8749-4F12776AE02C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="C11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>34</v>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{E020EE75-E187-4C2B-B76E-CBA9026E10D7}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{62BFAFEF-F4D9-4B4F-8438-ED6B1910AAB3}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{666C1F20-AD25-4247-8448-694F517F3ADD}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{8D4484CB-D258-4817-AF0C-0CDA7F807973}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{D4226753-749D-4F76-94CA-E027FF9EC69D}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{F5A9BB11-9BEC-4037-8B9A-7BE31F8661C2}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{E0F88E5B-CC95-4865-BC7B-CEEFECFA43E0}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{6265D4CE-EF3E-458E-8696-12E754212AD2}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{B1E78FB8-8776-4434-BADC-D3FE46B3BF53}"/>
-    <hyperlink ref="D10" r:id="rId10" xr:uid="{E9130E8D-FD40-4C40-A069-66B351BCE911}"/>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{9573F0C8-AB4D-4071-A548-D2FAD77DBA34}"/>
+    <hyperlink ref="D11" r:id="rId2" xr:uid="{A84777D8-3A09-45B0-BEA7-55CE4AE729D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>